<commit_message>
Various update. Beginning graphing
</commit_message>
<xml_diff>
--- a/tyre_models/modelling_metadata.xlsx
+++ b/tyre_models/modelling_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox\tyre_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C83B368-8AE7-49EE-896B-623F21E7AEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887912A7-8920-40CD-BB73-EF816F52CDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
   </bookViews>
@@ -248,9 +248,6 @@
     <t>6.2x20.0-14</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>2,3</t>
   </si>
   <si>
@@ -363,6 +360,9 @@
   </si>
   <si>
     <t>IDK</t>
+  </si>
+  <si>
+    <t>FS</t>
   </si>
 </sst>
 </file>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468A4279-5396-4636-97E1-217505AB1BD5}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>34</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>34</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>34</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>34</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>34</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>39</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>39</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>42</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>42</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>34</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>34</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>39</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>39</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>49</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>34</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>34</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>34</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>62</v>
@@ -1522,23 +1522,23 @@
         <v>16</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="4">
+        <v>7</v>
+      </c>
+      <c r="G21" s="3">
+        <v>7</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F21" s="4">
-        <v>7</v>
-      </c>
-      <c r="G21" s="3">
-        <v>7</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>56</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>20_Avon_7.0x16.0-10_ _7Rim.tir</v>
+        <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>29</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>62</v>
@@ -1558,7 +1558,7 @@
         <v>16</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F22" s="4">
         <v>8</v>
@@ -1567,14 +1567,14 @@
         <v>7</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>21_Avon_7.0x16.0-11_ _8Rim.tir</v>
+        <v>21_Avon_7.0x16.0-11_FS_8Rim.tir</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>29</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>62</v>
@@ -1594,7 +1594,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F23" s="4">
         <v>8</v>
@@ -1606,11 +1606,11 @@
         <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>22_Avon_8.2x20.0-13_ _8Rim.tir</v>
+        <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>29</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>62</v>
@@ -1630,7 +1630,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F24" s="4">
         <v>9</v>
@@ -1639,14 +1639,14 @@
         <v>7</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>23_Avon_8.2x20.0-14_ _9Rim.tir</v>
+        <v>23_Avon_8.2x20.0-14_FS_9Rim.tir</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>29</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>62</v>
@@ -1666,7 +1666,7 @@
         <v>16</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F25" s="4">
         <v>7</v>
@@ -1678,11 +1678,11 @@
         <v>53</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>24_Avon_7.2x20.0-13_ _7Rim.tir</v>
+        <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>29</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>62</v>
@@ -1702,7 +1702,7 @@
         <v>16</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F26" s="4">
         <v>8</v>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>25_Avon_7.2x20.0-13_ _8Rim.tir</v>
+        <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>29</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>62</v>
@@ -1738,7 +1738,7 @@
         <v>16</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F27" s="4">
         <v>6</v>
@@ -1750,11 +1750,11 @@
         <v>51</v>
       </c>
       <c r="I27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>26_Avon_6.2x20.0-13_ _6Rim.tir</v>
+        <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>29</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>62</v>
@@ -1774,7 +1774,7 @@
         <v>16</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F28" s="4">
         <v>7</v>
@@ -1786,11 +1786,11 @@
         <v>52</v>
       </c>
       <c r="I28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>27_Avon_6.2x20.0-14_ _7Rim.tir</v>
+        <v>27_Avon_6.2x20.0-14_FS_7Rim.tir</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>29</v>
@@ -1804,16 +1804,16 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J29" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Heaps of changes. Very proud
</commit_message>
<xml_diff>
--- a/tyre_models/modelling_metadata.xlsx
+++ b/tyre_models/modelling_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887912A7-8920-40CD-BB73-EF816F52CDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232E6250-9768-45D1-B71F-1F4345A54071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
   </bookViews>
@@ -152,9 +152,6 @@
     <t>16x6.0-10</t>
   </si>
   <si>
-    <t>18x6.0–10</t>
-  </si>
-  <si>
     <t>Goodyear</t>
   </si>
   <si>
@@ -363,6 +360,9 @@
   </si>
   <si>
     <t>FS</t>
+  </si>
+  <si>
+    <t>18x6.0-10</t>
   </si>
 </sst>
 </file>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468A4279-5396-4636-97E1-217505AB1BD5}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,7 +800,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>33</v>
@@ -818,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -850,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="2" t="str">
         <f>_xlfn.CONCAT( A2, "_", B2,"_",C2,"_",E2,"_",F2,"Rim.tir")</f>
@@ -862,7 +862,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>34</v>
@@ -886,7 +886,7 @@
         <v>6</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J3" s="2" t="str">
         <f t="shared" ref="J3:J29" si="0">_xlfn.CONCAT( A3, "_", B3,"_",C3,"_",E3,"_",F3,"Rim.tir")</f>
@@ -898,7 +898,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>34</v>
@@ -922,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -934,7 +934,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>34</v>
@@ -958,7 +958,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -970,13 +970,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="D6" s="4">
         <v>18</v>
@@ -998,7 +998,7 @@
       </c>
       <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>05_Hoosier_18x6.0–10_R20_6Rim.tir</v>
+        <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>29</v>
@@ -1006,13 +1006,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="D7" s="4">
         <v>18</v>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>06_Hoosier_18x6.0–10_R20_7Rim.tir</v>
+        <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>29</v>
@@ -1042,19 +1042,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="4">
         <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3">
         <v>6</v>
@@ -1078,19 +1078,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4">
         <v>18</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="3">
         <v>7</v>
@@ -1114,19 +1114,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D10" s="4">
         <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="3">
         <v>6</v>
@@ -1150,19 +1150,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D11" s="4">
         <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3">
         <v>7</v>
@@ -1186,13 +1186,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="4">
         <v>20.5</v>
@@ -1222,13 +1222,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="4">
         <v>20.5</v>
@@ -1258,19 +1258,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="4">
         <v>20</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="3">
         <v>7</v>
@@ -1294,19 +1294,19 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4">
         <v>20</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="3">
         <v>8</v>
@@ -1330,19 +1330,19 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="4">
         <v>16.14</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16" s="4">
         <v>7</v>
@@ -1351,10 +1351,10 @@
         <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1366,19 +1366,19 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="4">
         <v>16</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="4">
         <v>6</v>
@@ -1387,10 +1387,10 @@
         <v>8</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1402,19 +1402,19 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="4">
         <v>16</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="4">
         <v>7</v>
@@ -1423,10 +1423,10 @@
         <v>8</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1438,19 +1438,19 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4">
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F19" s="4">
         <v>8</v>
@@ -1459,10 +1459,10 @@
         <v>8</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1474,19 +1474,19 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="4">
         <v>16</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="4">
         <v>7</v>
@@ -1495,10 +1495,10 @@
         <v>8</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1510,19 +1510,19 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
         <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
       </c>
       <c r="D21" s="4">
         <v>16</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="4">
         <v>7</v>
@@ -1531,10 +1531,10 @@
         <v>7</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1546,19 +1546,19 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="4">
         <v>16</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F22" s="4">
         <v>8</v>
@@ -1567,10 +1567,10 @@
         <v>7</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1582,19 +1582,19 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="4">
         <v>16</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F23" s="4">
         <v>8</v>
@@ -1606,7 +1606,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1618,19 +1618,19 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="4">
         <v>16</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F24" s="4">
         <v>9</v>
@@ -1639,10 +1639,10 @@
         <v>7</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1654,19 +1654,19 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="4">
         <v>16</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F25" s="4">
         <v>7</v>
@@ -1675,10 +1675,10 @@
         <v>7</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1690,19 +1690,19 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="4">
         <v>16</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F26" s="4">
         <v>8</v>
@@ -1711,10 +1711,10 @@
         <v>7</v>
       </c>
       <c r="H26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1726,19 +1726,19 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="4">
         <v>16</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F27" s="4">
         <v>6</v>
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1762,19 +1762,19 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="4">
         <v>16</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F28" s="4">
         <v>7</v>
@@ -1783,10 +1783,10 @@
         <v>7</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1804,16 +1804,16 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" t="s">
-        <v>107</v>
-      </c>
       <c r="G29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J29" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
More work on tire selection
</commit_message>
<xml_diff>
--- a/tyre_models/modelling_metadata.xlsx
+++ b/tyre_models/modelling_metadata.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232E6250-9768-45D1-B71F-1F4345A54071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19B6326-DD8C-4293-BC7A-45A443AAC909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -777,19 +777,19 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.36328125" customWidth="1"/>
-    <col min="11" max="11" width="21.453125" customWidth="1"/>
+    <col min="1" max="3" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -824,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
@@ -860,7 +860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>79</v>
       </c>
@@ -896,7 +896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -932,7 +932,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>81</v>
       </c>
@@ -968,7 +968,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>82</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>83</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>84</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>85</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>86</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>87</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>88</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>89</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>90</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>92</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>93</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>94</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>95</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>96</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>97</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>98</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>99</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>100</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>101</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>102</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>103</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>104</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added unsprung mass for roudn 7,8,9
</commit_message>
<xml_diff>
--- a/tyre_models/modelling_metadata.xlsx
+++ b/tyre_models/modelling_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19B6326-DD8C-4293-BC7A-45A443AAC909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAA8D46-E68D-4F6D-8A3C-6F3F7CAE9C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
   <si>
     <t>Rim Width (in.)</t>
   </si>
@@ -227,24 +227,15 @@
     <t>7.0x16.0-10</t>
   </si>
   <si>
-    <t>7.0x16.0-11</t>
-  </si>
-  <si>
     <t>8.2x20.0-13</t>
   </si>
   <si>
-    <t>8.2x20.0-14</t>
-  </si>
-  <si>
     <t>7.2x20.0-13</t>
   </si>
   <si>
     <t>6.2x20.0-13</t>
   </si>
   <si>
-    <t>6.2x20.0-14</t>
-  </si>
-  <si>
     <t>2,3</t>
   </si>
   <si>
@@ -363,12 +354,21 @@
   </si>
   <si>
     <t>18x6.0-10</t>
+  </si>
+  <si>
+    <t>spring_rate</t>
+  </si>
+  <si>
+    <t>unsprung_mass (from Calspan Summary Tables)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -428,6 +428,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,25 +774,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468A4279-5396-4636-97E1-217505AB1BD5}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="1" max="3" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.453125" customWidth="1"/>
+    <col min="11" max="11" width="23.453125" customWidth="1"/>
+    <col min="12" max="12" width="18.6328125" customWidth="1"/>
+    <col min="13" max="13" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -818,15 +823,21 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -856,13 +867,17 @@
         <f>_xlfn.CONCAT( A2, "_", B2,"_",C2,"_",E2,"_",F2,"Rim.tir")</f>
         <v>01_Hoosier_16x7.5-10_R20_7Rim.tir</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="6">
+        <v>5.4204243999999999</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>34</v>
@@ -892,13 +907,17 @@
         <f t="shared" ref="J3:J29" si="0">_xlfn.CONCAT( A3, "_", B3,"_",C3,"_",E3,"_",F3,"Rim.tir")</f>
         <v>02_Hoosier_16x7.5-10_R20_8Rim.tir</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="6">
+        <v>5.5655738399999999</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>34</v>
@@ -928,13 +947,17 @@
         <f t="shared" si="0"/>
         <v>03_Hoosier_16x6.0-10_R20_6Rim.tir</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="6">
+        <v>5.0824983599999998</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>34</v>
@@ -964,19 +987,23 @@
         <f t="shared" si="0"/>
         <v>04_Hoosier_16x6.0-10_R20_7Rim.tir</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="6">
+        <v>5.3591894799999995</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D6" s="4">
         <v>18</v>
@@ -1000,19 +1027,23 @@
         <f t="shared" si="0"/>
         <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="6">
+        <v>5.5066068800000005</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" s="4">
         <v>18</v>
@@ -1036,13 +1067,17 @@
         <f t="shared" si="0"/>
         <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="6">
+        <v>5.7402067599999995</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>38</v>
@@ -1072,13 +1107,17 @@
         <f t="shared" si="0"/>
         <v>07_Goodyear_18.0x6.5-10_D0571_6Rim.tir</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="6">
+        <v>5.7061873599999995</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>38</v>
@@ -1108,13 +1147,17 @@
         <f t="shared" si="0"/>
         <v>08_Goodyear_18.0x6.5-10_D0571_7Rim.tir</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="6">
+        <v>6.0010221599999998</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>41</v>
@@ -1144,13 +1187,17 @@
         <f t="shared" si="0"/>
         <v>09_MRF_18x6-10_ZTD1_6Rim.tir</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="6">
+        <v>5.8921600799999991</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>41</v>
@@ -1180,13 +1227,17 @@
         <f t="shared" si="0"/>
         <v>10_MRF_18x6-10_ZTD1_7Rim.tir</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="6">
+        <v>6.1461715999999997</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>34</v>
@@ -1216,13 +1267,17 @@
         <f t="shared" si="0"/>
         <v>11_Hoosier_20.5x7-13_R20_7Rim.tir</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="6">
+        <v>13.66219104</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>34</v>
@@ -1252,13 +1307,17 @@
         <f t="shared" si="0"/>
         <v>12_Hoosier_20.5x7-13_R20_8Rim.tir</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="6">
+        <v>11.902254079999999</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>38</v>
@@ -1288,13 +1347,17 @@
         <f t="shared" si="0"/>
         <v>13_Goodyear_20.0x7-13_D2704_7Rim.tir</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="6">
+        <v>12.163069480000001</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>38</v>
@@ -1324,13 +1387,17 @@
         <f t="shared" si="0"/>
         <v>14_Goodyear_20.0x7-13_D2704_8Rim.tir</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="6">
+        <v>10.40086456</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>48</v>
@@ -1360,13 +1427,17 @@
         <f t="shared" si="0"/>
         <v>15_Continental_205x470R-13_FS43329_7Rim.tir</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="6">
+        <v>11.929469599999999</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
@@ -1396,13 +1467,17 @@
         <f t="shared" si="0"/>
         <v>16_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="6">
+        <v>5.1323934799999993</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>34</v>
@@ -1432,13 +1507,17 @@
         <f t="shared" si="0"/>
         <v>17_Hoosier_16.0x6.0-10_LCO_7Rim.tir</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="6">
+        <v>5.3047584399999996</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>34</v>
@@ -1468,13 +1547,17 @@
         <f t="shared" si="0"/>
         <v>18_Hoosier_16.0x7.5-10_LCO_8Rim.tir</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="6">
+        <v>5.6971155200000005</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>34</v>
@@ -1504,13 +1587,17 @@
         <f t="shared" si="0"/>
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="6">
+        <v>5.7515465599999995</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>61</v>
@@ -1522,7 +1609,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F21" s="4">
         <v>7</v>
@@ -1531,7 +1618,7 @@
         <v>7</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>55</v>
@@ -1540,25 +1627,29 @@
         <f t="shared" si="0"/>
         <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="6">
+        <v>5.5179466799999997</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="4">
         <v>16</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F22" s="4">
         <v>8</v>
@@ -1567,34 +1658,38 @@
         <v>7</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>55</v>
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>21_Avon_7.0x16.0-11_FS_8Rim.tir</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21_Avon_7.0x16.0-10_FS_8Rim.tir</v>
+      </c>
+      <c r="K22" s="6">
+        <v>5.6086650799999997</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="4">
         <v>16</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F23" s="4">
         <v>8</v>
@@ -1606,31 +1701,35 @@
         <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="6">
+        <v>11.93854144</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" s="4">
         <v>16</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F24" s="4">
         <v>9</v>
@@ -1639,34 +1738,38 @@
         <v>7</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>23_Avon_8.2x20.0-14_FS_9Rim.tir</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23_Avon_8.2x20.0-13_FS_9Rim.tir</v>
+      </c>
+      <c r="K24" s="6">
+        <v>11.981632679999999</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D25" s="4">
         <v>16</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F25" s="4">
         <v>7</v>
@@ -1678,31 +1781,35 @@
         <v>52</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="6">
+        <v>13.458074640000001</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D26" s="4">
         <v>16</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F26" s="4">
         <v>8</v>
@@ -1720,25 +1827,29 @@
         <f t="shared" si="0"/>
         <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="6">
+        <v>12.02925984</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D27" s="4">
         <v>16</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F27" s="4">
         <v>6</v>
@@ -1750,31 +1861,35 @@
         <v>50</v>
       </c>
       <c r="I27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
       </c>
-      <c r="K27" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="6">
+        <v>10.763738160000001</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D28" s="4">
         <v>16</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F28" s="4">
         <v>7</v>
@@ -1786,17 +1901,21 @@
         <v>51</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>27_Avon_6.2x20.0-14_FS_7Rim.tir</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27_Avon_6.2x20.0-13_FS_7Rim.tir</v>
+      </c>
+      <c r="K28" s="6">
+        <v>13.140560239999999</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1804,27 +1923,29 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>28_Hoosier_Something_LCO_IDKRim.tir</v>
       </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="K1:K1048576">
+  <conditionalFormatting sqref="M1:M1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",K1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("yes",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First pass of succesful tyre ranking
</commit_message>
<xml_diff>
--- a/tyre_models/modelling_metadata.xlsx
+++ b/tyre_models/modelling_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAA8D46-E68D-4F6D-8A3C-6F3F7CAE9C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EABECB-C710-4DC8-8454-38F80B1FD725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
   </bookViews>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468A4279-5396-4636-97E1-217505AB1BD5}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,7 +794,7 @@
     <col min="13" max="13" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Added fake combined model
</commit_message>
<xml_diff>
--- a/tyre_models/modelling_metadata.xlsx
+++ b/tyre_models/modelling_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox_new\tyre_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EABECB-C710-4DC8-8454-38F80B1FD725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AA7A64-2A89-455C-9D5F-A95BC75BE615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D90D173-2EA1-4E28-9D60-3DFDF8560CA4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="111">
   <si>
     <t>Rim Width (in.)</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>unsprung_mass (from Calspan Summary Tables)</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>29</t>
   </si>
 </sst>
 </file>
@@ -412,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -432,6 +441,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468A4279-5396-4636-97E1-217505AB1BD5}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,7 +1598,7 @@
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
       </c>
       <c r="K20" s="6">
-        <v>5.7515465599999995</v>
+        <v>5.7515465600000004</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
@@ -1940,6 +1950,42 @@
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="4">
+        <v>16</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="4">
+        <v>6</v>
+      </c>
+      <c r="G30" s="3">
+        <v>99</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" s="2" t="str">
+        <f t="shared" ref="J30" si="1">_xlfn.CONCAT( A30, "_", B30,"_",C30,"_",E30,"_",F30,"Rim.tir")</f>
+        <v>29_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
+      </c>
+      <c r="K30" s="6">
+        <v>5.1323934799999993</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>